<commit_message>
4.3 export detail excel
</commit_message>
<xml_diff>
--- a/API/Resources/Template/SortSumReport.xlsx
+++ b/API/Resources/Template/SortSumReport.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <t>Brand</t>
   </si>
@@ -163,10 +163,6 @@
   <si>
     <t>Cancel priting 
 quantity</t>
-  </si>
-  <si>
-    <t>Storage scan 
-Qty</t>
   </si>
 </sst>
 </file>
@@ -541,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,13 +565,12 @@
     <col min="18" max="18" width="10.28515625" style="4" customWidth="1"/>
     <col min="19" max="19" width="11.7109375" style="4" customWidth="1"/>
     <col min="20" max="20" width="10.7109375" style="4" customWidth="1"/>
-    <col min="21" max="21" width="14.5703125" style="4" customWidth="1"/>
-    <col min="22" max="22" width="12.85546875" style="4" customWidth="1"/>
-    <col min="23" max="23" width="16.42578125" style="4" customWidth="1"/>
-    <col min="24" max="16384" width="9.140625" style="4"/>
+    <col min="21" max="21" width="12.85546875" style="4" customWidth="1"/>
+    <col min="22" max="22" width="16.42578125" style="4" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="6" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" s="6" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
@@ -637,16 +632,13 @@
         <v>40</v>
       </c>
       <c r="U1" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="V1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="W1" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
@@ -708,12 +700,9 @@
         <v>22</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="V2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="W2" s="4" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
done 4.3 storage sum report
</commit_message>
<xml_diff>
--- a/API/Resources/Template/SortSumReport.xlsx
+++ b/API/Resources/Template/SortSumReport.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <t>Brand</t>
   </si>
@@ -163,10 +163,6 @@
   <si>
     <t>Cancel priting 
 quantity</t>
-  </si>
-  <si>
-    <t>Storage scan 
-Qty</t>
   </si>
 </sst>
 </file>
@@ -541,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,13 +565,12 @@
     <col min="18" max="18" width="10.28515625" style="4" customWidth="1"/>
     <col min="19" max="19" width="11.7109375" style="4" customWidth="1"/>
     <col min="20" max="20" width="10.7109375" style="4" customWidth="1"/>
-    <col min="21" max="21" width="14.5703125" style="4" customWidth="1"/>
-    <col min="22" max="22" width="12.85546875" style="4" customWidth="1"/>
-    <col min="23" max="23" width="16.42578125" style="4" customWidth="1"/>
-    <col min="24" max="16384" width="9.140625" style="4"/>
+    <col min="21" max="21" width="12.85546875" style="4" customWidth="1"/>
+    <col min="22" max="22" width="16.42578125" style="4" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="6" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" s="6" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
@@ -637,16 +632,13 @@
         <v>40</v>
       </c>
       <c r="U1" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="V1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="W1" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
@@ -708,12 +700,9 @@
         <v>22</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="V2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="W2" s="4" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>